<commit_message>
my first commit to local
</commit_message>
<xml_diff>
--- a/ComCast_CRM_Framework/data/testdata.xlsx
+++ b/ComCast_CRM_Framework/data/testdata.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SDET_25_26\ComCast_CRM_Framework\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18520" windowHeight="5860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12360" windowHeight="5860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="org" sheetId="1" r:id="rId1"/>
     <sheet name="contact" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>TC_ID</t>
   </si>
@@ -103,9 +99,6 @@
   </si>
   <si>
     <t>9888888898</t>
-  </si>
-  <si>
-    <t>Ty_Banglore</t>
   </si>
   <si>
     <t>conatctName</t>
@@ -548,7 +541,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -598,7 +591,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -609,7 +602,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>

</xml_diff>